<commit_message>
fix : 강화 2->3
</commit_message>
<xml_diff>
--- a/RawData/Unit_Data.xlsx
+++ b/RawData/Unit_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grays\Desktop\Project\Unity\OIlNamProject\RawData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{427B29EC-9455-4033-9BB7-6FC4EC5D48E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41F219AF-6F48-4091-8DF9-4156D4F62532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="35250" yWindow="2310" windowWidth="20010" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="44">
   <si>
     <t>Name</t>
   </si>
@@ -47,9 +47,6 @@
     <t>모든지 열심히 합니다.</t>
   </si>
   <si>
-    <t>초보자.gif</t>
-  </si>
-  <si>
     <t>전사 1</t>
   </si>
   <si>
@@ -62,18 +59,12 @@
     <t>부족장입니다.</t>
   </si>
   <si>
-    <t>전사 2.gif</t>
-  </si>
-  <si>
     <t>전사 3</t>
   </si>
   <si>
     <t>조금 느리지만 힘이 쎈 족장입니다.</t>
   </si>
   <si>
-    <t>전사 3.gif</t>
-  </si>
-  <si>
     <t>궁수 1</t>
   </si>
   <si>
@@ -86,18 +77,12 @@
     <t>날쎈 궁수입니다.</t>
   </si>
   <si>
-    <t>궁수 2.gif</t>
-  </si>
-  <si>
     <t>궁수 3</t>
   </si>
   <si>
     <t>궁수 중엔 내가 제일 쎕니다.</t>
   </si>
   <si>
-    <t>궁수 3.gif</t>
-  </si>
-  <si>
     <t>마법사 1</t>
   </si>
   <si>
@@ -110,16 +95,10 @@
     <t>25년 동안 모솔입니다.</t>
   </si>
   <si>
-    <t>마법사 2.gif</t>
-  </si>
-  <si>
     <t>마법사 3</t>
   </si>
   <si>
     <t>30년 동안 모솔입니다.</t>
-  </si>
-  <si>
-    <t>마법사 3.gif</t>
   </si>
   <si>
     <r>
@@ -276,13 +255,14 @@
   </si>
   <si>
     <t>Archer0</t>
-  </si>
-  <si>
-    <t>Archer0</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Human0</t>
+  </si>
+  <si>
+    <t>Mage0</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -853,7 +833,7 @@
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -872,16 +852,16 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
@@ -890,22 +870,22 @@
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -917,10 +897,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>3</v>
@@ -938,10 +918,10 @@
         <v>1</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -953,10 +933,10 @@
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>3</v>
@@ -974,10 +954,10 @@
         <v>1</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -988,10 +968,10 @@
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>3</v>
@@ -1009,10 +989,10 @@
         <v>1</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -1023,13 +1003,13 @@
         <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>6</v>
       </c>
       <c r="G5" s="2">
         <v>27</v>
@@ -1044,10 +1024,10 @@
         <v>2</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -1058,13 +1038,13 @@
         <v>2</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="G6" s="2">
         <v>30</v>
@@ -1079,10 +1059,10 @@
         <v>3</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -1093,13 +1073,13 @@
         <v>3</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G7" s="2">
         <v>31.6</v>
@@ -1114,10 +1094,10 @@
         <v>4</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
@@ -1128,13 +1108,13 @@
         <v>1</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G8" s="2">
         <v>13.32</v>
@@ -1149,10 +1129,10 @@
         <v>5</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
@@ -1163,13 +1143,13 @@
         <v>2</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G9" s="2">
         <v>14</v>
@@ -1184,10 +1164,10 @@
         <v>6</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
@@ -1198,13 +1178,13 @@
         <v>3</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G10" s="2">
         <v>15</v>
@@ -1219,10 +1199,10 @@
         <v>7</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
@@ -1233,13 +1213,13 @@
         <v>1</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G11" s="2">
         <v>25.6</v>
@@ -1254,10 +1234,10 @@
         <v>8</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
@@ -1268,13 +1248,13 @@
         <v>2</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="G12" s="2">
         <v>26.7</v>
@@ -1289,10 +1269,10 @@
         <v>9</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
@@ -1303,13 +1283,13 @@
         <v>3</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="G13" s="2">
         <v>27</v>
@@ -1324,10 +1304,10 @@
         <v>10</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>